<commit_message>
listo la base de datos y scripts sql
</commit_message>
<xml_diff>
--- a/docs/tablas SQL.xlsx
+++ b/docs/tablas SQL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\loopBack\lbCopaAmerica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\loopBack\lbcopa-america\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0">
+    <comment ref="I22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="76">
   <si>
     <t>Paises</t>
   </si>
@@ -270,9 +270,6 @@
     <t>nu_goles2</t>
   </si>
   <si>
-    <t>lf_partido</t>
-  </si>
-  <si>
     <t>Penaltis</t>
   </si>
   <si>
@@ -307,6 +304,18 @@
   </si>
   <si>
     <t>nu_golesContra</t>
+  </si>
+  <si>
+    <t>hr_partido</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>id_persona_var</t>
+  </si>
+  <si>
+    <t>dt_partido</t>
   </si>
 </sst>
 </file>
@@ -352,7 +361,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +701,7 @@
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="2"/>
     </row>
@@ -728,7 +737,7 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
         <v>2</v>
@@ -766,7 +775,7 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
@@ -792,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -828,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -852,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -926,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
         <v>2</v>
@@ -952,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L9" t="s">
         <v>2</v>
@@ -978,7 +987,7 @@
         <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
         <v>2</v>
@@ -998,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L11" t="s">
         <v>2</v>
@@ -1019,8 +1028,14 @@
       <c r="H12" t="s">
         <v>2</v>
       </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
       <c r="K12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L12" t="s">
         <v>2</v>
@@ -1049,8 +1064,14 @@
       <c r="H13" t="s">
         <v>2</v>
       </c>
+      <c r="I13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" t="s">
+        <v>73</v>
+      </c>
       <c r="K13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L13" t="s">
         <v>2</v>
@@ -1081,10 +1102,6 @@
       <c r="H14" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
@@ -1099,12 +1116,6 @@
       <c r="F15" t="s">
         <v>3</v>
       </c>
-      <c r="I15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1120,12 +1131,10 @@
         <v>50</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" t="s">
-        <v>2</v>
-      </c>
+      <c r="I16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
@@ -1145,7 +1154,7 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="J17" t="s">
         <v>2</v>
@@ -1164,6 +1173,12 @@
       <c r="H18" t="s">
         <v>2</v>
       </c>
+      <c r="I18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
@@ -1178,6 +1193,12 @@
       <c r="H19" t="s">
         <v>2</v>
       </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
@@ -1190,10 +1211,6 @@
       <c r="H20" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
@@ -1202,12 +1219,6 @@
       <c r="D21" t="s">
         <v>2</v>
       </c>
-      <c r="I21" t="s">
-        <v>43</v>
-      </c>
-      <c r="J21" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
@@ -1216,25 +1227,31 @@
       <c r="D22" t="s">
         <v>3</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
         <v>44</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J24" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E13:F13"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I22:J22"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A5:B5"/>
@@ -1242,6 +1259,14 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
listo todos los controladeres
</commit_message>
<xml_diff>
--- a/docs/tablas SQL.xlsx
+++ b/docs/tablas SQL.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="81">
   <si>
     <t>Paises</t>
   </si>
@@ -126,9 +126,6 @@
     <t>tx_Grupo</t>
   </si>
   <si>
-    <t>tx_ligar</t>
-  </si>
-  <si>
     <t>tx_nombre</t>
   </si>
   <si>
@@ -234,21 +231,6 @@
     <t>id_equipo</t>
   </si>
   <si>
-    <t>DetalleEquipo</t>
-  </si>
-  <si>
-    <t>TipoPersonaTecnica</t>
-  </si>
-  <si>
-    <t>PersonasTecnicas</t>
-  </si>
-  <si>
-    <t>DetallesGrupos</t>
-  </si>
-  <si>
-    <t>DetalleSedes</t>
-  </si>
-  <si>
     <t>Partidos</t>
   </si>
   <si>
@@ -276,9 +258,6 @@
     <t>nu_goles</t>
   </si>
   <si>
-    <t>TipoPartidos</t>
-  </si>
-  <si>
     <t>id_tipoPartidos</t>
   </si>
   <si>
@@ -316,6 +295,42 @@
   </si>
   <si>
     <t>dt_partido</t>
+  </si>
+  <si>
+    <t>DetEquipo</t>
+  </si>
+  <si>
+    <t>id_det_equipo</t>
+  </si>
+  <si>
+    <t>DetGrupos</t>
+  </si>
+  <si>
+    <t>id_det_grupo</t>
+  </si>
+  <si>
+    <t>DetSedes</t>
+  </si>
+  <si>
+    <t>id_det_sedes</t>
+  </si>
+  <si>
+    <t>TipPersonaTec</t>
+  </si>
+  <si>
+    <t>TipPartido</t>
+  </si>
+  <si>
+    <t>PersonasTec</t>
+  </si>
+  <si>
+    <t>id_penaltis</t>
+  </si>
+  <si>
+    <t>id_puntos</t>
+  </si>
+  <si>
+    <t>tx_lugar</t>
   </si>
 </sst>
 </file>
@@ -667,11 +682,12 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -689,19 +705,19 @@
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="L1" s="2"/>
     </row>
@@ -725,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
@@ -737,7 +753,7 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
         <v>2</v>
@@ -751,10 +767,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -763,19 +779,19 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
@@ -783,25 +799,25 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -813,31 +829,31 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -849,22 +865,22 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
         <v>8</v>
@@ -881,19 +897,19 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
         <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
         <v>2</v>
@@ -913,29 +929,29 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J8" t="s">
         <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L8" t="s">
         <v>2</v>
@@ -943,25 +959,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="J9" t="s">
         <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L9" t="s">
         <v>2</v>
@@ -969,45 +985,51 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="I10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J11" t="s">
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="L11" t="s">
         <v>2</v>
@@ -1015,27 +1037,27 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2"/>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="J12" t="s">
         <v>2</v>
       </c>
       <c r="K12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="L12" t="s">
         <v>2</v>
@@ -1043,7 +1065,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -1054,24 +1076,20 @@
       <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="2"/>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" t="s">
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="L13" t="s">
         <v>2</v>
@@ -1079,7 +1097,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -1090,102 +1108,112 @@
       <c r="D14" t="s">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
         <v>31</v>
       </c>
-      <c r="F14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>37</v>
-      </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
         <v>1</v>
@@ -1194,55 +1222,73 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="D20" s="2"/>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D22" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
       <c r="I23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
         <v>43</v>
-      </c>
-      <c r="J23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I24" t="s">
-        <v>44</v>
       </c>
       <c r="J24" t="s">
         <v>3</v>
@@ -1250,7 +1296,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A1:B1"/>
@@ -1263,10 +1313,6 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Primera carga de datos y pruebas
</commit_message>
<xml_diff>
--- a/docs/tablas SQL.xlsx
+++ b/docs/tablas SQL.xlsx
@@ -367,7 +367,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,6 +377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,10 +399,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -682,7 +691,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,14 +705,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
@@ -824,10 +833,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>18</v>
       </c>
@@ -1036,14 +1045,14 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="3"/>
       <c r="G12" t="s">
         <v>33</v>
       </c>
@@ -1229,10 +1238,10 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="3"/>
       <c r="E20" t="s">
         <v>36</v>
       </c>
@@ -1296,11 +1305,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E18:F18"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A1:B1"/>
@@ -1313,6 +1317,11 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>